<commit_message>
Test 2 Adding Files Modified
</commit_message>
<xml_diff>
--- a/CartaTiemposRev00.xlsx
+++ b/CartaTiemposRev00.xlsx
@@ -16,6 +16,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Cambio en Linea 1 Hoja 1</t>
+  </si>
+  <si>
+    <t>Cambio en Columna 2</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,12 +393,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Adding Excel Modification at Samuel's Branch
</commit_message>
<xml_diff>
--- a/CartaTiemposRev00.xlsx
+++ b/CartaTiemposRev00.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Cambio en Linea 1 Hoja 1</t>
   </si>
   <si>
     <t>Cambio en Columna 2</t>
+  </si>
+  <si>
+    <t>Cambio Branch de Samuel</t>
   </si>
 </sst>
 </file>
@@ -395,8 +399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -421,4 +425,27 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>